<commit_message>
[Shubham] October updated code
</commit_message>
<xml_diff>
--- a/data/excel/BrandInformation.xlsx
+++ b/data/excel/BrandInformation.xlsx
@@ -1,14 +1,17 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26529"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26626"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DFA1CA53-CCAA-493B-A217-E70C6D761977}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E22A9126-4E7E-4D53-9D89-59A20C6BA99E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="5" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="6" r:id="rId2"/>
+    <sheet name="Sheet3" sheetId="7" r:id="rId3"/>
+    <sheet name="Sheet4" sheetId="8" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -31,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="222" uniqueCount="82">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="600" uniqueCount="101">
   <si>
     <t>TestCaseId</t>
   </si>
@@ -277,6 +280,63 @@
   </si>
   <si>
     <t>Test 10</t>
+  </si>
+  <si>
+    <t>A,B,C,D,E,F,G,H,I,J,K,L,M,N,O,P,Q,R,S,T,U,V,W,X,Y,Z</t>
+  </si>
+  <si>
+    <t>KG</t>
+  </si>
+  <si>
+    <t>CORPORATE</t>
+  </si>
+  <si>
+    <t>SpiceJet</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Refundable till </t>
+  </si>
+  <si>
+    <t>15 days</t>
+  </si>
+  <si>
+    <t>16 days</t>
+  </si>
+  <si>
+    <t>17 days</t>
+  </si>
+  <si>
+    <t>18 days</t>
+  </si>
+  <si>
+    <t>D:\\OneDrive - QuadLabs Technologies Pvt Ltd (HQ - Gurgaon)\\Desktop\\carry on baggage.png</t>
+  </si>
+  <si>
+    <t>D:\\OneDrive - QuadLabs Technologies Pvt Ltd (HQ - Gurgaon)\\Desktop\\Refundable 2.png</t>
+  </si>
+  <si>
+    <t>Baggage carry on</t>
+  </si>
+  <si>
+    <t>Baggage Check In</t>
+  </si>
+  <si>
+    <t>D:\\OneDrive - QuadLabs Technologies Pvt Ltd (HQ - Gurgaon)\\Desktop\\check in baggage 2.png</t>
+  </si>
+  <si>
+    <t>D:\\OneDrive - QuadLabs Technologies Pvt Ltd (HQ - Gurgaon)\\Desktop\\meal.png</t>
+  </si>
+  <si>
+    <t>KIQty</t>
+  </si>
+  <si>
+    <t>Credit Card Required</t>
+  </si>
+  <si>
+    <t>Check in baggage,Hand baggage,Credit Card Required</t>
+  </si>
+  <si>
+    <t>15KG,2KG,Yes</t>
   </si>
 </sst>
 </file>
@@ -650,8 +710,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2580B81A-822A-488B-ABC2-C12B5D035DA4}">
   <dimension ref="A1:V11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C25" sqref="C25"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:XFD2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1483,4 +1543,1498 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId21"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{877D712E-DEBF-40E4-A74D-298670F67BC0}">
+  <dimension ref="A1:V17"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:XFD2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="10.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="71.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="7" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="23.28515625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="14" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10.28515625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="10.5703125" bestFit="1" customWidth="1"/>
+    <col min="9" max="10" width="9.140625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="15.85546875" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="47.140625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="11.42578125" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="16.42578125" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="14.7109375" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="13.42578125" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="16.28515625" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="87.140625" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="16.140625" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="12.85546875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="J1" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="K1" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="L1" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="M1" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="N1" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="O1" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="P1" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="Q1" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="R1" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="S1" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="T1" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="U1" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="V1" s="1" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="2" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A2" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="E2" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="F2" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="G2" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="H2" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="I2" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="J2" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="K2" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="L2" s="3">
+        <v>26</v>
+      </c>
+      <c r="M2" s="3" t="s">
+        <v>82</v>
+      </c>
+      <c r="N2" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="O2" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="P2" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="Q2" s="3">
+        <v>15</v>
+      </c>
+      <c r="R2" s="3" t="s">
+        <v>83</v>
+      </c>
+      <c r="S2" s="3" t="s">
+        <v>93</v>
+      </c>
+      <c r="T2" s="3" t="s">
+        <v>91</v>
+      </c>
+      <c r="U2" s="3">
+        <v>1</v>
+      </c>
+      <c r="V2" s="3" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="3" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A3" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="E3" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="F3" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="G3" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="H3" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="I3" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="J3" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="K3" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="L3" s="3">
+        <v>26</v>
+      </c>
+      <c r="M3" s="3" t="s">
+        <v>82</v>
+      </c>
+      <c r="N3" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="O3" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="P3" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="Q3" s="3">
+        <v>16</v>
+      </c>
+      <c r="R3" s="3" t="s">
+        <v>83</v>
+      </c>
+      <c r="S3" s="3" t="s">
+        <v>93</v>
+      </c>
+      <c r="T3" s="3" t="s">
+        <v>91</v>
+      </c>
+      <c r="U3" s="3">
+        <v>1</v>
+      </c>
+      <c r="V3" s="3" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="4" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A4" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="D4" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="E4" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="F4" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="G4" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="H4" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="I4" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="J4" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="K4" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="L4" s="3">
+        <v>26</v>
+      </c>
+      <c r="M4" s="3" t="s">
+        <v>82</v>
+      </c>
+      <c r="N4" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="O4" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="P4" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="Q4" s="3">
+        <v>17</v>
+      </c>
+      <c r="R4" s="3" t="s">
+        <v>83</v>
+      </c>
+      <c r="S4" s="3" t="s">
+        <v>93</v>
+      </c>
+      <c r="T4" s="3" t="s">
+        <v>91</v>
+      </c>
+      <c r="U4" s="3">
+        <v>1</v>
+      </c>
+      <c r="V4" s="3" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="5" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A5" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="D5" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="E5" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="F5" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="G5" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="H5" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="I5" s="3" t="s">
+        <v>85</v>
+      </c>
+      <c r="J5" s="3" t="s">
+        <v>85</v>
+      </c>
+      <c r="K5" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="L5" s="3">
+        <v>26</v>
+      </c>
+      <c r="M5" s="3" t="s">
+        <v>82</v>
+      </c>
+      <c r="N5" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="O5" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="P5" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="Q5" s="3">
+        <v>18</v>
+      </c>
+      <c r="R5" s="3" t="s">
+        <v>83</v>
+      </c>
+      <c r="S5" s="3" t="s">
+        <v>93</v>
+      </c>
+      <c r="T5" s="3" t="s">
+        <v>91</v>
+      </c>
+      <c r="U5" s="3">
+        <v>1</v>
+      </c>
+      <c r="V5" s="3" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="6" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A6" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="D6" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="E6" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="F6" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="G6" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="H6" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="I6" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="J6" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="K6" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="L6" s="3">
+        <v>26</v>
+      </c>
+      <c r="M6" s="3" t="s">
+        <v>82</v>
+      </c>
+      <c r="N6" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="O6" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="P6" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="Q6" s="3" t="s">
+        <v>86</v>
+      </c>
+      <c r="R6" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="S6" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="T6" s="3" t="s">
+        <v>92</v>
+      </c>
+      <c r="U6" s="3">
+        <v>1</v>
+      </c>
+      <c r="V6" s="3" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="7" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A7" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C7" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="D7" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="E7" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="F7" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="G7" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="H7" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="I7" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="J7" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="K7" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="L7" s="3">
+        <v>26</v>
+      </c>
+      <c r="M7" s="3" t="s">
+        <v>82</v>
+      </c>
+      <c r="N7" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="O7" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="P7" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="Q7" s="3" t="s">
+        <v>86</v>
+      </c>
+      <c r="R7" s="3" t="s">
+        <v>88</v>
+      </c>
+      <c r="S7" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="T7" s="3" t="s">
+        <v>92</v>
+      </c>
+      <c r="U7" s="3">
+        <v>1</v>
+      </c>
+      <c r="V7" s="3" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="8" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A8" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="B8" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C8" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="D8" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="E8" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="F8" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="G8" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="H8" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="I8" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="J8" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="K8" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="L8" s="3">
+        <v>26</v>
+      </c>
+      <c r="M8" s="3" t="s">
+        <v>82</v>
+      </c>
+      <c r="N8" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="O8" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="P8" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="Q8" s="3" t="s">
+        <v>86</v>
+      </c>
+      <c r="R8" s="3" t="s">
+        <v>89</v>
+      </c>
+      <c r="S8" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="T8" s="3" t="s">
+        <v>92</v>
+      </c>
+      <c r="U8" s="3">
+        <v>1</v>
+      </c>
+      <c r="V8" s="3" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="9" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A9" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="B9" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C9" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="D9" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="E9" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="F9" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="G9" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="H9" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="I9" s="3" t="s">
+        <v>85</v>
+      </c>
+      <c r="J9" s="3" t="s">
+        <v>85</v>
+      </c>
+      <c r="K9" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="L9" s="3">
+        <v>26</v>
+      </c>
+      <c r="M9" s="3" t="s">
+        <v>82</v>
+      </c>
+      <c r="N9" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="O9" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="P9" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="Q9" s="3" t="s">
+        <v>86</v>
+      </c>
+      <c r="R9" s="3" t="s">
+        <v>90</v>
+      </c>
+      <c r="S9" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="T9" s="3" t="s">
+        <v>92</v>
+      </c>
+      <c r="U9" s="3">
+        <v>1</v>
+      </c>
+      <c r="V9" s="3" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="10" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A10" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="B10" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C10" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="D10" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="E10" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="F10" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="G10" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="H10" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="I10" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="J10" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="K10" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="L10" s="3">
+        <v>26</v>
+      </c>
+      <c r="M10" s="3" t="s">
+        <v>82</v>
+      </c>
+      <c r="N10" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="O10" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="P10" s="3" t="s">
+        <v>94</v>
+      </c>
+      <c r="Q10" s="3">
+        <v>15</v>
+      </c>
+      <c r="R10" s="3" t="s">
+        <v>83</v>
+      </c>
+      <c r="S10" s="3" t="s">
+        <v>94</v>
+      </c>
+      <c r="T10" s="3" t="s">
+        <v>95</v>
+      </c>
+      <c r="U10" s="3">
+        <v>1</v>
+      </c>
+      <c r="V10" s="3" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="11" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A11" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="B11" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C11" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="D11" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="E11" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="F11" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="G11" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="H11" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="I11" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="J11" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="K11" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="L11" s="3">
+        <v>26</v>
+      </c>
+      <c r="M11" s="3" t="s">
+        <v>82</v>
+      </c>
+      <c r="N11" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="O11" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="P11" s="3" t="s">
+        <v>94</v>
+      </c>
+      <c r="Q11" s="3">
+        <v>16</v>
+      </c>
+      <c r="R11" s="3" t="s">
+        <v>83</v>
+      </c>
+      <c r="S11" s="3" t="s">
+        <v>94</v>
+      </c>
+      <c r="T11" s="3" t="s">
+        <v>95</v>
+      </c>
+      <c r="U11" s="3">
+        <v>1</v>
+      </c>
+      <c r="V11" s="3" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="12" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A12" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="B12" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C12" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="D12" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="E12" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="F12" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="G12" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="H12" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="I12" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="J12" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="K12" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="L12" s="3">
+        <v>26</v>
+      </c>
+      <c r="M12" s="3" t="s">
+        <v>82</v>
+      </c>
+      <c r="N12" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="O12" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="P12" s="3" t="s">
+        <v>94</v>
+      </c>
+      <c r="Q12" s="3">
+        <v>17</v>
+      </c>
+      <c r="R12" s="3" t="s">
+        <v>83</v>
+      </c>
+      <c r="S12" s="3" t="s">
+        <v>94</v>
+      </c>
+      <c r="T12" s="3" t="s">
+        <v>95</v>
+      </c>
+      <c r="U12" s="3">
+        <v>1</v>
+      </c>
+      <c r="V12" s="3" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="13" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A13" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="B13" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C13" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="D13" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="E13" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="F13" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="G13" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="H13" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="I13" s="3" t="s">
+        <v>85</v>
+      </c>
+      <c r="J13" s="3" t="s">
+        <v>85</v>
+      </c>
+      <c r="K13" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="L13" s="3">
+        <v>26</v>
+      </c>
+      <c r="M13" s="3" t="s">
+        <v>82</v>
+      </c>
+      <c r="N13" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="O13" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="P13" s="3" t="s">
+        <v>94</v>
+      </c>
+      <c r="Q13" s="3">
+        <v>18</v>
+      </c>
+      <c r="R13" s="3" t="s">
+        <v>83</v>
+      </c>
+      <c r="S13" s="3" t="s">
+        <v>94</v>
+      </c>
+      <c r="T13" s="3" t="s">
+        <v>95</v>
+      </c>
+      <c r="U13" s="3">
+        <v>1</v>
+      </c>
+      <c r="V13" s="3" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="14" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A14" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="B14" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C14" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="D14" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="E14" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="F14" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="G14" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="H14" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="I14" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="J14" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="K14" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="L14" s="3">
+        <v>26</v>
+      </c>
+      <c r="M14" s="3" t="s">
+        <v>82</v>
+      </c>
+      <c r="N14" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="O14" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="P14" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="Q14" s="3" t="s">
+        <v>86</v>
+      </c>
+      <c r="R14" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="S14" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="T14" s="3" t="s">
+        <v>96</v>
+      </c>
+      <c r="U14" s="3">
+        <v>1</v>
+      </c>
+      <c r="V14" s="3" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="15" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A15" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="B15" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C15" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="D15" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="E15" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="F15" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="G15" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="H15" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="I15" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="J15" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="K15" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="L15" s="3">
+        <v>26</v>
+      </c>
+      <c r="M15" s="3" t="s">
+        <v>82</v>
+      </c>
+      <c r="N15" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="O15" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="P15" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="Q15" s="3" t="s">
+        <v>86</v>
+      </c>
+      <c r="R15" s="3" t="s">
+        <v>88</v>
+      </c>
+      <c r="S15" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="T15" s="3" t="s">
+        <v>96</v>
+      </c>
+      <c r="U15" s="3">
+        <v>1</v>
+      </c>
+      <c r="V15" s="3" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="16" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A16" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="B16" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C16" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="D16" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="E16" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="F16" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="G16" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="H16" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="I16" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="J16" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="K16" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="L16" s="3">
+        <v>26</v>
+      </c>
+      <c r="M16" s="3" t="s">
+        <v>82</v>
+      </c>
+      <c r="N16" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="O16" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="P16" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="Q16" s="3" t="s">
+        <v>86</v>
+      </c>
+      <c r="R16" s="3" t="s">
+        <v>89</v>
+      </c>
+      <c r="S16" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="T16" s="3" t="s">
+        <v>96</v>
+      </c>
+      <c r="U16" s="3">
+        <v>1</v>
+      </c>
+      <c r="V16" s="3" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="17" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A17" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="B17" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C17" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="D17" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="E17" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="F17" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="G17" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="H17" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="I17" s="3" t="s">
+        <v>85</v>
+      </c>
+      <c r="J17" s="3" t="s">
+        <v>85</v>
+      </c>
+      <c r="K17" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="L17" s="3">
+        <v>26</v>
+      </c>
+      <c r="M17" s="3" t="s">
+        <v>82</v>
+      </c>
+      <c r="N17" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="O17" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="P17" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="Q17" s="3" t="s">
+        <v>86</v>
+      </c>
+      <c r="R17" s="3" t="s">
+        <v>90</v>
+      </c>
+      <c r="S17" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="T17" s="3" t="s">
+        <v>96</v>
+      </c>
+      <c r="U17" s="3">
+        <v>1</v>
+      </c>
+      <c r="V17" s="3" t="s">
+        <v>84</v>
+      </c>
+    </row>
+  </sheetData>
+  <dataValidations count="8">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="P2:P17" xr:uid="{12B60AD7-597D-4C78-B8C3-3C827C01D73E}">
+      <formula1>"Baggage Carry On,Baggage Check In,Refundable,Cancellation Amount,Exchange Amount,No Show Amount,Meal Description,In Flight Intertainment"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="N2:N17" xr:uid="{6AF97EB9-282B-4C9B-8CC3-EDB11203643B}">
+      <formula1>"Domestic,International"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="K2:K17" xr:uid="{9FD73CCB-F785-4C42-A33D-15BA45726D73}">
+      <formula1>"Economy,Premium Economy,Business,First"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="J2:J17" xr:uid="{7399BBAF-4975-427F-AD44-E55C6C858B27}">
+      <formula1>"Air India,Indigo,Vistara,SpiceJet,Akasa Air,Emirates,Air Asia"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H2:H17" xr:uid="{15D91E97-7EA6-442C-B741-E3B0473F978A}">
+      <formula1>"Laxmi@123,Quad@720"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G2:G17" xr:uid="{6DEDABE3-92BF-4CDF-B550-5F14C500DC34}">
+      <formula1>"saurav_at"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F2:F17" xr:uid="{2524584C-2830-4BF9-8B2A-EEF4CDFFA948}">
+      <formula1>"at"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B2:B17" xr:uid="{CC1BD6B9-8661-4F94-AC59-FE64090CA3EB}">
+      <formula1>"Positive,Negative"</formula1>
+    </dataValidation>
+  </dataValidations>
+  <hyperlinks>
+    <hyperlink ref="G2" r:id="rId1" display="shubham.natkar@quadlabs.com" xr:uid="{E2B559C8-3088-4155-8A07-7A267524387A}"/>
+    <hyperlink ref="H2" r:id="rId2" display="Shekhar123@" xr:uid="{97DA0B16-4120-4C8F-A66C-8BF3E6BA575E}"/>
+    <hyperlink ref="G3" r:id="rId3" display="shubham.natkar@quadlabs.com" xr:uid="{18CC48A2-CBA1-4442-8419-708B99771052}"/>
+    <hyperlink ref="H3" r:id="rId4" display="Shekhar123@" xr:uid="{739D986E-053A-493E-8237-1B568C3479C4}"/>
+    <hyperlink ref="G4" r:id="rId5" display="shubham.natkar@quadlabs.com" xr:uid="{C152895C-907D-40F4-B7FD-3DC9F6BC1B22}"/>
+    <hyperlink ref="H4" r:id="rId6" display="Shekhar123@" xr:uid="{745828C3-9655-4902-B4D7-FDAEA9AD2F53}"/>
+    <hyperlink ref="G5" r:id="rId7" display="shubham.natkar@quadlabs.com" xr:uid="{ADE2875F-27EA-41ED-A3BC-8155AA7F63EA}"/>
+    <hyperlink ref="H5" r:id="rId8" display="Shekhar123@" xr:uid="{690B48C1-B771-44A3-8C45-8484826624FD}"/>
+    <hyperlink ref="G6" r:id="rId9" display="shubham.natkar@quadlabs.com" xr:uid="{742ABEF8-EB5C-4EB3-B3CD-419FBE9BC71D}"/>
+    <hyperlink ref="H6" r:id="rId10" display="Shekhar123@" xr:uid="{39F50034-5FCB-40E0-BB3C-EDA832693642}"/>
+    <hyperlink ref="G7" r:id="rId11" display="shubham.natkar@quadlabs.com" xr:uid="{E521AD2E-6F60-4B53-9147-E4FDAA3E3539}"/>
+    <hyperlink ref="H7" r:id="rId12" display="Shekhar123@" xr:uid="{FE2A9AC0-6E01-49FE-B72C-8FCBF53F8816}"/>
+    <hyperlink ref="G8" r:id="rId13" display="shubham.natkar@quadlabs.com" xr:uid="{80397269-FED9-4D54-89C3-6224B24EA7EE}"/>
+    <hyperlink ref="H8" r:id="rId14" display="Shekhar123@" xr:uid="{D1EBB077-AD24-406D-B8CB-DC8893C5B168}"/>
+    <hyperlink ref="G9" r:id="rId15" display="shubham.natkar@quadlabs.com" xr:uid="{38488B7D-8726-4CB0-9D0E-ED214EB600EE}"/>
+    <hyperlink ref="H9" r:id="rId16" display="Shekhar123@" xr:uid="{769C38E0-ABC2-4388-9C11-FE31D1FF2901}"/>
+    <hyperlink ref="G10" r:id="rId17" display="shubham.natkar@quadlabs.com" xr:uid="{6A16F5D2-1D24-41B0-B561-50A42D0C0DBB}"/>
+    <hyperlink ref="H10" r:id="rId18" display="Shekhar123@" xr:uid="{BFFB0641-60DE-439A-A5C1-29C0E21B51BC}"/>
+    <hyperlink ref="G11" r:id="rId19" display="shubham.natkar@quadlabs.com" xr:uid="{4436A0B2-8A88-462E-A1AB-478A8CF9B284}"/>
+    <hyperlink ref="H11" r:id="rId20" display="Shekhar123@" xr:uid="{EBC7CA90-4512-4DBE-835E-1AF208E2EF37}"/>
+    <hyperlink ref="G12" r:id="rId21" display="shubham.natkar@quadlabs.com" xr:uid="{66AEBF01-74BB-4C0B-AE2D-094AD701AD94}"/>
+    <hyperlink ref="H12" r:id="rId22" display="Shekhar123@" xr:uid="{CE51148E-5EBE-4775-B7A2-8CD6212EA170}"/>
+    <hyperlink ref="G13" r:id="rId23" display="shubham.natkar@quadlabs.com" xr:uid="{E7F4A65C-2B58-4813-8D2A-46A9C1BF3C47}"/>
+    <hyperlink ref="H13" r:id="rId24" display="Shekhar123@" xr:uid="{469B34FB-8353-4E94-92DF-FB5C1318FBB3}"/>
+    <hyperlink ref="G14" r:id="rId25" display="shubham.natkar@quadlabs.com" xr:uid="{D09375C5-DF68-44F5-B586-7360725A9388}"/>
+    <hyperlink ref="H14" r:id="rId26" display="Shekhar123@" xr:uid="{AEAE4690-4105-4BDD-B09C-66B41317610C}"/>
+    <hyperlink ref="G15" r:id="rId27" display="shubham.natkar@quadlabs.com" xr:uid="{F9DB191E-B1BA-44B3-B736-D6D42BFD1E26}"/>
+    <hyperlink ref="H15" r:id="rId28" display="Shekhar123@" xr:uid="{3491ABC3-B84C-4E7F-AFCB-446E0A9D27AA}"/>
+    <hyperlink ref="G16" r:id="rId29" display="shubham.natkar@quadlabs.com" xr:uid="{93B75C91-0C20-4C9F-8AF3-BDD594D49242}"/>
+    <hyperlink ref="H16" r:id="rId30" display="Shekhar123@" xr:uid="{896D9627-9BDA-4B90-B1D3-D0E1800E2F7B}"/>
+    <hyperlink ref="G17" r:id="rId31" display="shubham.natkar@quadlabs.com" xr:uid="{E35B9065-FD88-4FA3-95C7-CF4D8B8D1C90}"/>
+    <hyperlink ref="H17" r:id="rId32" display="Shekhar123@" xr:uid="{31EC5B15-945A-49C9-9CB8-C2F2C6CB06AB}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{372E727A-CAD1-4C8E-B772-0AB921756487}">
+  <dimension ref="A1:W2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="M1" workbookViewId="0">
+      <selection activeCell="R10" sqref="R10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="10.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="71.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="7" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="23.28515625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="14" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10.28515625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="10.5703125" bestFit="1" customWidth="1"/>
+    <col min="9" max="10" width="7.7109375" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="15.85546875" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="47.140625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="11.42578125" bestFit="1" customWidth="1"/>
+    <col min="16" max="17" width="13.42578125" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="87.140625" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="16.140625" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="12.85546875" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="12.85546875" customWidth="1"/>
+    <col min="22" max="22" width="49.28515625" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="13.140625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="J1" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="K1" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="L1" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="M1" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="N1" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="O1" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="P1" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="Q1" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="R1" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="S1" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="T1" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="U1" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="V1" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="W1" s="2" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="2" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A2" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="E2" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="F2" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="G2" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="H2" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="I2" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="J2" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="K2" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="L2" s="3">
+        <v>26</v>
+      </c>
+      <c r="M2" s="3" t="s">
+        <v>82</v>
+      </c>
+      <c r="N2" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="O2" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="P2" s="3">
+        <v>15</v>
+      </c>
+      <c r="Q2" s="3" t="s">
+        <v>83</v>
+      </c>
+      <c r="R2" s="3" t="s">
+        <v>91</v>
+      </c>
+      <c r="S2" s="3">
+        <v>1</v>
+      </c>
+      <c r="T2" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="U2" s="3">
+        <v>3</v>
+      </c>
+      <c r="V2" s="3" t="s">
+        <v>99</v>
+      </c>
+      <c r="W2" s="3" t="s">
+        <v>100</v>
+      </c>
+    </row>
+  </sheetData>
+  <dataValidations count="7">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B2" xr:uid="{5E5DA670-A324-42F5-93CA-32E9E8A05265}">
+      <formula1>"Positive,Negative"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F2" xr:uid="{72A00D1B-A1C5-4881-8D40-A5A7E783C1C8}">
+      <formula1>"at"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G2" xr:uid="{6589B780-7E82-4E16-B41F-766D1EEE3356}">
+      <formula1>"saurav_at"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H2" xr:uid="{5AFBB740-621D-481A-9CA2-E8C084193A5B}">
+      <formula1>"Laxmi@123,Quad@720"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="J2" xr:uid="{61B149F2-683E-47F4-9225-851BA6EDD40A}">
+      <formula1>"Air India,Indigo,Vistara,SpiceJet,Akasa Air,Emirates,Air Asia"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="K2" xr:uid="{AC2F5824-24D0-4028-8F0D-DB0746420770}">
+      <formula1>"Economy,Premium Economy,Business,First"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="N2" xr:uid="{02F07404-6AA3-4E43-8D19-F0366AAC6C19}">
+      <formula1>"Domestic,International"</formula1>
+    </dataValidation>
+  </dataValidations>
+  <hyperlinks>
+    <hyperlink ref="G2" r:id="rId1" display="shubham.natkar@quadlabs.com" xr:uid="{DCDAEC92-D54A-436F-84D9-3A7383207AB0}"/>
+    <hyperlink ref="H2" r:id="rId2" display="Shekhar123@" xr:uid="{FEA0A227-7236-42AB-BC66-D0B77872FAFE}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{79ECD744-C2DC-43CC-9D5E-E40C78FCFCDA}">
+  <dimension ref="A1:A2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="16.28515625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A1" s="2" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A2" s="3" t="s">
+        <v>98</v>
+      </c>
+    </row>
+  </sheetData>
+  <dataValidations count="1">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A2" xr:uid="{395EF70B-D321-48BE-A3B3-F3F45A2ECE3C}">
+      <formula1>"Beverage,Refreshment,Check in baggage,Carry on baggage,Hand baggage,Fast Track,Credit Card Required,Meal,Changeable,Changeable ticket,Miles Earned,Seats,Refunds,Mileage Upgrade,Wireless,Food,In Flight Entertainment,Chauffeur Drive,Lounge Access,Lounges"</formula1>
+    </dataValidation>
+  </dataValidations>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>